<commit_message>
Fill created overwatch table with user input data
</commit_message>
<xml_diff>
--- a/outputs/planilhaSobreaviso.xlsx
+++ b/outputs/planilhaSobreaviso.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alicia.santos\Documents\PROJETOS\RPA002_BRB_SOBREAVISO_SPREAD_Carolina Schuch\CODIGO\RPA002_BRB_SOBREAVISO_SPREAD_CarolinaSchuch\outputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972D59F-7AB5-466E-9A5D-AB377FC31C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr fullPrecision="1" calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="73">
   <si>
     <t>Dia</t>
   </si>
@@ -72,36 +66,39 @@
   <si>
     <t>Alicia</t>
   </si>
+  <si>
+    <t>359.969.368-44</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,26 +110,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
+  <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
@@ -439,24 +436,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="B1" view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.41796875" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.84765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" customHeight="1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -491,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -526,7 +524,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -561,7 +559,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -596,7 +594,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -631,7 +629,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -666,7 +664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -701,7 +699,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -736,7 +734,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -771,7 +769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -806,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -841,7 +839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -876,7 +874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -911,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -946,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -981,9 +979,570 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G16">
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>19</v>
+      </c>
+      <c r="K16">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G18">
+        <v>19</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1">
+        <v>6</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>17</v>
+      </c>
+      <c r="K20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1">
+        <v>6</v>
+      </c>
+      <c r="F21" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G21">
+        <v>19</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6</v>
+      </c>
+      <c r="F23" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G23">
+        <v>19</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6</v>
+      </c>
+      <c r="F24" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>17</v>
+      </c>
+      <c r="K24">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1">
+        <v>6</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G25">
+        <v>19</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <v>12</v>
+      </c>
+      <c r="K25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6</v>
+      </c>
+      <c r="F26" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G27">
+        <v>19</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1">
+        <v>6</v>
+      </c>
+      <c r="F28" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>7</v>
+      </c>
+      <c r="J28">
+        <v>17</v>
+      </c>
+      <c r="K28">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6</v>
+      </c>
+      <c r="F29" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G29">
+        <v>19</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>12</v>
+      </c>
+      <c r="K29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6</v>
+      </c>
+      <c r="F30" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>7</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2022</v>
+      </c>
+      <c r="G31">
+        <v>19</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+  <extLst/>
 </worksheet>
 </file>
</xml_diff>